<commit_message>
Reference authorities by index and not name
</commit_message>
<xml_diff>
--- a/testdata/sample.xlsx
+++ b/testdata/sample.xlsx
@@ -1928,8 +1928,8 @@
     </row>
     <row r="8" ht="80.35" customHeight="1">
       <c r="A8" s="2"/>
-      <c r="B8" t="s" s="2">
-        <v>8</v>
+      <c r="B8" s="2">
+        <v>1</v>
       </c>
       <c r="C8" t="s" s="2">
         <v>20</v>
@@ -1937,8 +1937,8 @@
       <c r="D8" t="s" s="2">
         <v>21</v>
       </c>
-      <c r="E8" t="s" s="2">
-        <v>3</v>
+      <c r="E8" s="2">
+        <v>1</v>
       </c>
       <c r="F8" t="s" s="2">
         <v>22</v>

</xml_diff>

<commit_message>
Pluralized appropriate column names
</commit_message>
<xml_diff>
--- a/testdata/sample.xlsx
+++ b/testdata/sample.xlsx
@@ -53,7 +53,7 @@
     <t>Actions</t>
   </si>
   <si>
-    <t>State authority approached</t>
+    <t>State authorities approached</t>
   </si>
   <si>
     <t>Complaint to state authority</t>
@@ -62,7 +62,7 @@
     <t>Response from state authority</t>
   </si>
   <si>
-    <t>International authority approached</t>
+    <t>International authorities approached</t>
   </si>
   <si>
     <t>Complaint to international authority</t>
@@ -218,7 +218,7 @@
     <t>Type code</t>
   </si>
   <si>
-    <t>Rights Violation</t>
+    <t>Rights Violations</t>
   </si>
   <si>
     <t>Torture</t>

</xml_diff>

<commit_message>
Add field for rights violations to be listed in excel doc
</commit_message>
<xml_diff>
--- a/testdata/sample.xlsx
+++ b/testdata/sample.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="110">
   <si>
     <t>International Authorities</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>Perpetrators</t>
+  </si>
+  <si>
+    <t>Rights violations</t>
   </si>
   <si>
     <t>Event 1</t>
@@ -1675,7 +1678,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W45"/>
+  <dimension ref="A1:X45"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1704,7 +1707,8 @@
     <col min="21" max="21" width="9.05469" style="1" customWidth="1"/>
     <col min="22" max="22" width="9.05469" style="1" customWidth="1"/>
     <col min="23" max="23" width="9.05469" style="1" customWidth="1"/>
-    <col min="24" max="256" width="9.05469" style="1" customWidth="1"/>
+    <col min="24" max="24" width="9.05469" style="1" customWidth="1"/>
+    <col min="25" max="256" width="9.05469" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="32.35" customHeight="1">
@@ -1737,6 +1741,7 @@
       <c r="U1" s="3"/>
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
     </row>
     <row r="2" ht="44.35" customHeight="1">
       <c r="A2" s="2"/>
@@ -1766,6 +1771,7 @@
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
     </row>
     <row r="3" ht="44.35" customHeight="1">
       <c r="A3" s="3"/>
@@ -1795,6 +1801,7 @@
       <c r="U3" s="3"/>
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
     </row>
     <row r="4" ht="32.35" customHeight="1">
       <c r="A4" t="s" s="2">
@@ -1826,6 +1833,7 @@
       <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
     </row>
     <row r="5" ht="44.35" customHeight="1">
       <c r="A5" s="3"/>
@@ -1855,6 +1863,7 @@
       <c r="U5" s="3"/>
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
     </row>
     <row r="6" ht="68.35" customHeight="1">
       <c r="A6" s="3"/>
@@ -1884,6 +1893,7 @@
       <c r="U6" s="3"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
     </row>
     <row r="7" ht="56.35" customHeight="1">
       <c r="A7" t="s" s="2">
@@ -1925,6 +1935,7 @@
       <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
     </row>
     <row r="8" ht="80.35" customHeight="1">
       <c r="A8" s="2"/>
@@ -1964,6 +1975,7 @@
       <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
     </row>
     <row r="9" ht="20.35" customHeight="1">
       <c r="A9" t="s" s="2">
@@ -1997,6 +2009,7 @@
       <c r="U9" s="3"/>
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
     </row>
     <row r="10" ht="56.35" customHeight="1">
       <c r="A10" s="3"/>
@@ -2028,6 +2041,7 @@
       <c r="U10" s="3"/>
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
     </row>
     <row r="11" ht="104.35" customHeight="1">
       <c r="A11" s="3"/>
@@ -2059,6 +2073,7 @@
       <c r="U11" s="3"/>
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
     </row>
     <row r="12" ht="68.35" customHeight="1">
       <c r="A12" s="3"/>
@@ -2090,6 +2105,7 @@
       <c r="U12" s="3"/>
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
+      <c r="X12" s="3"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
       <c r="A13" t="s" s="2">
@@ -2119,6 +2135,7 @@
       <c r="U13" s="3"/>
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
       <c r="A14" s="3"/>
@@ -2146,6 +2163,7 @@
       <c r="U14" s="3"/>
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
     </row>
     <row r="15" ht="32.35" customHeight="1">
       <c r="A15" s="3"/>
@@ -2173,6 +2191,7 @@
       <c r="U15" s="3"/>
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
     </row>
     <row r="16" ht="20.35" customHeight="1">
       <c r="A16" s="3"/>
@@ -2200,6 +2219,7 @@
       <c r="U16" s="3"/>
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
     </row>
     <row r="17" ht="20.35" customHeight="1">
       <c r="A17" s="3"/>
@@ -2227,6 +2247,7 @@
       <c r="U17" s="3"/>
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
     </row>
     <row r="18" ht="20.35" customHeight="1">
       <c r="A18" t="s" s="2">
@@ -2260,6 +2281,7 @@
       <c r="U18" s="3"/>
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
     </row>
     <row r="19" ht="32.35" customHeight="1">
       <c r="A19" s="3"/>
@@ -2291,6 +2313,7 @@
       <c r="U19" s="3"/>
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
     </row>
     <row r="20" ht="32.35" customHeight="1">
       <c r="A20" s="3"/>
@@ -2322,6 +2345,7 @@
       <c r="U20" s="3"/>
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
     </row>
     <row r="21" ht="32.35" customHeight="1">
       <c r="A21" s="3"/>
@@ -2353,6 +2377,7 @@
       <c r="U21" s="3"/>
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
     </row>
     <row r="22" ht="32.35" customHeight="1">
       <c r="A22" t="s" s="2">
@@ -2400,6 +2425,7 @@
       <c r="U22" s="3"/>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
+      <c r="X22" s="3"/>
     </row>
     <row r="23" ht="32.35" customHeight="1">
       <c r="A23" s="2"/>
@@ -2445,6 +2471,7 @@
       <c r="U23" s="3"/>
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
     </row>
     <row r="24" ht="44.35" customHeight="1">
       <c r="A24" s="3"/>
@@ -2490,6 +2517,7 @@
       <c r="U24" s="3"/>
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
     </row>
     <row r="25" ht="56.35" customHeight="1">
       <c r="A25" s="3"/>
@@ -2533,6 +2561,7 @@
       <c r="U25" s="3"/>
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
     </row>
     <row r="26" ht="32.35" customHeight="1">
       <c r="A26" t="s" s="2">
@@ -2562,6 +2591,7 @@
       <c r="U26" s="3"/>
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
     </row>
     <row r="27" ht="20.35" customHeight="1">
       <c r="A27" s="3"/>
@@ -2589,6 +2619,7 @@
       <c r="U27" s="3"/>
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
     </row>
     <row r="28" ht="20.35" customHeight="1">
       <c r="A28" s="3"/>
@@ -2616,6 +2647,7 @@
       <c r="U28" s="3"/>
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
+      <c r="X28" s="3"/>
     </row>
     <row r="29" ht="20.35" customHeight="1">
       <c r="A29" s="3"/>
@@ -2643,6 +2675,7 @@
       <c r="U29" s="3"/>
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
+      <c r="X29" s="3"/>
     </row>
     <row r="30" ht="32.35" customHeight="1">
       <c r="A30" t="s" s="2">
@@ -2674,6 +2707,7 @@
       <c r="U30" s="3"/>
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
+      <c r="X30" s="3"/>
     </row>
     <row r="31" ht="128.35" customHeight="1">
       <c r="A31" s="3"/>
@@ -2703,6 +2737,7 @@
       <c r="U31" s="3"/>
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
+      <c r="X31" s="3"/>
     </row>
     <row r="32" ht="80.35" customHeight="1">
       <c r="A32" s="3"/>
@@ -2732,6 +2767,7 @@
       <c r="U32" s="3"/>
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
+      <c r="X32" s="3"/>
     </row>
     <row r="33" ht="20.35" customHeight="1">
       <c r="A33" t="s" s="2">
@@ -2763,6 +2799,7 @@
       <c r="U33" s="3"/>
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
+      <c r="X33" s="3"/>
     </row>
     <row r="34" ht="32.35" customHeight="1">
       <c r="A34" s="3"/>
@@ -2792,6 +2829,7 @@
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
+      <c r="X34" s="3"/>
     </row>
     <row r="35" ht="20.35" customHeight="1">
       <c r="A35" s="3"/>
@@ -2821,6 +2859,7 @@
       <c r="U35" s="3"/>
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
+      <c r="X35" s="3"/>
     </row>
     <row r="36" ht="20.35" customHeight="1">
       <c r="A36" t="s" s="2">
@@ -2850,6 +2889,7 @@
       <c r="U36" s="3"/>
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
+      <c r="X36" s="3"/>
     </row>
     <row r="37" ht="32.35" customHeight="1">
       <c r="A37" s="3"/>
@@ -2877,6 +2917,7 @@
       <c r="U37" s="3"/>
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
+      <c r="X37" s="3"/>
     </row>
     <row r="38" ht="20.35" customHeight="1">
       <c r="A38" s="3"/>
@@ -2904,6 +2945,7 @@
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
+      <c r="X38" s="3"/>
     </row>
     <row r="39" ht="20.35" customHeight="1">
       <c r="A39" s="3"/>
@@ -2931,6 +2973,7 @@
       <c r="U39" s="3"/>
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
+      <c r="X39" s="3"/>
     </row>
     <row r="40" ht="20.35" customHeight="1">
       <c r="A40" t="s" s="2">
@@ -2964,6 +3007,7 @@
       <c r="U40" s="3"/>
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
+      <c r="X40" s="3"/>
     </row>
     <row r="41" ht="32.35" customHeight="1">
       <c r="A41" s="2"/>
@@ -2995,6 +3039,7 @@
       <c r="U41" s="3"/>
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
+      <c r="X41" s="3"/>
     </row>
     <row r="42" ht="56.35" customHeight="1">
       <c r="A42" t="s" s="2">
@@ -3066,20 +3111,23 @@
       <c r="W42" t="s" s="2">
         <v>101</v>
       </c>
+      <c r="X42" t="s" s="2">
+        <v>102</v>
+      </c>
     </row>
     <row r="43" ht="68.35" customHeight="1">
       <c r="A43" s="2"/>
       <c r="B43" t="s" s="2">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C43" t="s" s="2">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D43" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E43" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F43" s="5">
         <v>40460</v>
@@ -3135,13 +3183,16 @@
       <c r="W43" s="2">
         <v>3</v>
       </c>
+      <c r="X43" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="44" ht="20.35" customHeight="1">
       <c r="A44" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C44" t="s" s="2">
         <v>19</v>
@@ -3166,11 +3217,12 @@
       <c r="U44" s="3"/>
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
+      <c r="X44" s="3"/>
     </row>
     <row r="45" ht="44.35" customHeight="1">
       <c r="A45" s="2"/>
       <c r="B45" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C45" s="2">
         <v>1</v>
@@ -3195,6 +3247,7 @@
       <c r="U45" s="3"/>
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
+      <c r="X45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Make organisations reference locations by id
</commit_message>
<xml_diff>
--- a/testdata/sample.xlsx
+++ b/testdata/sample.xlsx
@@ -89,61 +89,61 @@
     <t>1, 3</t>
   </si>
   <si>
+    <t>Professions</t>
+  </si>
+  <si>
+    <t>Jounalist</t>
+  </si>
+  <si>
+    <t>Software developer</t>
+  </si>
+  <si>
+    <t>Politician</t>
+  </si>
+  <si>
+    <t>Military</t>
+  </si>
+  <si>
+    <t>Locations</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Montreal, QC, Canada</t>
+  </si>
+  <si>
+    <t>Toronto, ON, Canada</t>
+  </si>
+  <si>
+    <t>London, England</t>
+  </si>
+  <si>
+    <t>Secret Court</t>
+  </si>
+  <si>
     <t>Organisations</t>
   </si>
   <si>
-    <t>Locations</t>
-  </si>
-  <si>
     <t>The Tor Project</t>
   </si>
   <si>
     <t>Builds anonymity software  such as Tor</t>
   </si>
   <si>
-    <t>Montreal, QC, Canada</t>
-  </si>
-  <si>
     <t>The Guardian</t>
   </si>
   <si>
     <t>A reputable news organisation that has published numerous Snowden documents.</t>
   </si>
   <si>
-    <t>London, England</t>
-  </si>
-  <si>
     <t>American Governemnt</t>
   </si>
   <si>
     <t>The government of the United States of America</t>
-  </si>
-  <si>
-    <t>Washington D.C., United States of America</t>
-  </si>
-  <si>
-    <t>Professions</t>
-  </si>
-  <si>
-    <t>Jounalist</t>
-  </si>
-  <si>
-    <t>Software developer</t>
-  </si>
-  <si>
-    <t>Politician</t>
-  </si>
-  <si>
-    <t>Military</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Toronto, ON, Canada</t>
   </si>
   <si>
     <t>Actors</t>
@@ -1678,7 +1678,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X45"/>
+  <dimension ref="A1:X46"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1984,12 +1984,8 @@
       <c r="B9" t="s" s="2">
         <v>1</v>
       </c>
-      <c r="C9" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="D9" t="s" s="2">
-        <v>26</v>
-      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -2011,17 +2007,13 @@
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
     </row>
-    <row r="10" ht="56.35" customHeight="1">
+    <row r="10" ht="20.35" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" t="s" s="2">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s" s="2">
-        <v>29</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
@@ -2043,17 +2035,13 @@
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
     </row>
-    <row r="11" ht="104.35" customHeight="1">
+    <row r="11" ht="32.35" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s" s="2">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s" s="2">
-        <v>32</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
@@ -2075,17 +2063,13 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
     </row>
-    <row r="12" ht="68.35" customHeight="1">
+    <row r="12" ht="20.35" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" t="s" s="2">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s" s="2">
-        <v>35</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
@@ -2108,11 +2092,9 @@
       <c r="X12" s="3"/>
     </row>
     <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" t="s" s="2">
-        <v>36</v>
-      </c>
+      <c r="A13" s="3"/>
       <c r="B13" t="s" s="2">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -2138,12 +2120,18 @@
       <c r="X13" s="3"/>
     </row>
     <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" s="3"/>
+      <c r="A14" t="s" s="2">
+        <v>30</v>
+      </c>
       <c r="B14" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+        <v>1</v>
+      </c>
+      <c r="C14" t="s" s="2">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s" s="2">
+        <v>32</v>
+      </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
@@ -2168,10 +2156,14 @@
     <row r="15" ht="32.35" customHeight="1">
       <c r="A15" s="3"/>
       <c r="B15" t="s" s="2">
-        <v>38</v>
-      </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="C15" s="4">
+        <v>45.5505849</v>
+      </c>
+      <c r="D15" s="4">
+        <v>-73.60223164000119</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
@@ -2193,13 +2185,17 @@
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
     </row>
-    <row r="16" ht="20.35" customHeight="1">
+    <row r="16" ht="32.35" customHeight="1">
       <c r="A16" s="3"/>
       <c r="B16" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="C16" s="4">
+        <v>43.67368315</v>
+      </c>
+      <c r="D16" s="4">
+        <v>-79.3798433925311</v>
+      </c>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -2221,13 +2217,17 @@
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
     </row>
-    <row r="17" ht="20.35" customHeight="1">
+    <row r="17" ht="32.35" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
+        <v>35</v>
+      </c>
+      <c r="C17" s="4">
+        <v>51.5073219</v>
+      </c>
+      <c r="D17" s="4">
+        <v>-0.1276474</v>
+      </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -2249,18 +2249,16 @@
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
     </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" t="s" s="2">
-        <v>26</v>
-      </c>
+    <row r="18" ht="21.95" customHeight="1">
+      <c r="A18" s="3"/>
       <c r="B18" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D18" t="s" s="2">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4">
+        <v>0</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -2283,16 +2281,18 @@
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" ht="32.35" customHeight="1">
-      <c r="A19" s="3"/>
+    <row r="19" ht="20.35" customHeight="1">
+      <c r="A19" t="s" s="2">
+        <v>37</v>
+      </c>
       <c r="B19" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="C19" s="4">
-        <v>45.5505849</v>
-      </c>
-      <c r="D19" s="4">
-        <v>-73.60223164000119</v>
+        <v>1</v>
+      </c>
+      <c r="C19" t="s" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s" s="2">
+        <v>30</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -2315,16 +2315,16 @@
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" ht="32.35" customHeight="1">
+    <row r="20" ht="56.35" customHeight="1">
       <c r="A20" s="3"/>
       <c r="B20" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="C20" s="4">
-        <v>43.67368315</v>
-      </c>
-      <c r="D20" s="4">
-        <v>-79.3798433925311</v>
+        <v>38</v>
+      </c>
+      <c r="C20" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="D20" s="2">
+        <v>1</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -2347,16 +2347,16 @@
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
     </row>
-    <row r="21" ht="32.35" customHeight="1">
+    <row r="21" ht="104.35" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" t="s" s="2">
-        <v>32</v>
-      </c>
-      <c r="C21" s="4">
-        <v>51.5073219</v>
-      </c>
-      <c r="D21" s="4">
-        <v>-0.1276474</v>
+        <v>40</v>
+      </c>
+      <c r="C21" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D21" s="2">
+        <v>3</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -2379,40 +2379,24 @@
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
     </row>
-    <row r="22" ht="32.35" customHeight="1">
-      <c r="A22" t="s" s="2">
-        <v>44</v>
-      </c>
+    <row r="22" ht="68.35" customHeight="1">
+      <c r="A22" s="3"/>
       <c r="B22" t="s" s="2">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C22" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="D22" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="E22" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="F22" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G22" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="H22" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="I22" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="J22" t="s" s="2">
-        <v>36</v>
-      </c>
-      <c r="K22" t="s" s="2">
-        <v>26</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="D22" s="2">
+        <v>4</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
@@ -2428,38 +2412,40 @@
       <c r="X22" s="3"/>
     </row>
     <row r="23" ht="32.35" customHeight="1">
-      <c r="A23" s="2"/>
+      <c r="A23" t="s" s="2">
+        <v>44</v>
+      </c>
       <c r="B23" t="s" s="2">
-        <v>51</v>
-      </c>
-      <c r="C23" s="5">
-        <v>29962</v>
+        <v>1</v>
+      </c>
+      <c r="C23" t="s" s="2">
+        <v>45</v>
       </c>
       <c r="D23" t="s" s="2">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E23" t="s" s="2">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G23" t="s" s="2">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="I23" s="2">
-        <v>2</v>
-      </c>
-      <c r="J23" s="2">
-        <v>1</v>
-      </c>
-      <c r="K23" s="2">
-        <v>2</v>
-      </c>
-      <c r="L23" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="I23" t="s" s="2">
+        <v>37</v>
+      </c>
+      <c r="J23" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="K23" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
@@ -2473,39 +2459,39 @@
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
     </row>
-    <row r="24" ht="44.35" customHeight="1">
-      <c r="A24" s="3"/>
+    <row r="24" ht="32.35" customHeight="1">
+      <c r="A24" s="2"/>
       <c r="B24" t="s" s="2">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C24" s="5">
-        <v>26774</v>
+        <v>29962</v>
       </c>
       <c r="D24" t="s" s="2">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E24" t="s" s="2">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G24" t="s" s="2">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="H24" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="I24" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="J24" t="s" s="2">
-        <v>61</v>
+        <v>55</v>
+      </c>
+      <c r="I24" s="2">
+        <v>2</v>
+      </c>
+      <c r="J24" s="2">
+        <v>1</v>
       </c>
       <c r="K24" s="2">
-        <v>1</v>
-      </c>
-      <c r="L24" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="L24" s="2"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
@@ -2519,36 +2505,38 @@
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
     </row>
-    <row r="25" ht="56.35" customHeight="1">
+    <row r="25" ht="44.35" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" t="s" s="2">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C25" s="5">
-        <v>17502</v>
+        <v>26774</v>
       </c>
       <c r="D25" t="s" s="2">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E25" t="s" s="2">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G25" t="s" s="2">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="I25" s="2">
-        <v>3</v>
-      </c>
-      <c r="J25" s="2">
-        <v>4</v>
-      </c>
-      <c r="K25" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="I25" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="J25" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1</v>
+      </c>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
@@ -2563,21 +2551,35 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" ht="32.35" customHeight="1">
-      <c r="A26" t="s" s="2">
-        <v>66</v>
-      </c>
+    <row r="26" ht="56.35" customHeight="1">
+      <c r="A26" s="3"/>
       <c r="B26" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="C26" s="5">
+        <v>17502</v>
+      </c>
+      <c r="D26" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="E26" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="F26" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="G26" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="H26" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="I26" s="2">
+        <v>3</v>
+      </c>
+      <c r="J26" s="2">
+        <v>4</v>
+      </c>
       <c r="K26" s="3"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
@@ -2593,10 +2595,12 @@
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" ht="20.35" customHeight="1">
-      <c r="A27" s="3"/>
-      <c r="B27" s="2">
-        <v>1</v>
+    <row r="27" ht="32.35" customHeight="1">
+      <c r="A27" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="B27" t="s" s="2">
+        <v>67</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -2624,7 +2628,7 @@
     <row r="28" ht="20.35" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -2652,7 +2656,7 @@
     <row r="29" ht="20.35" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2677,16 +2681,12 @@
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
     </row>
-    <row r="30" ht="32.35" customHeight="1">
-      <c r="A30" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="B30" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s" s="2">
-        <v>2</v>
-      </c>
+    <row r="30" ht="20.35" customHeight="1">
+      <c r="A30" s="3"/>
+      <c r="B30" s="2">
+        <v>3</v>
+      </c>
+      <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -2709,13 +2709,15 @@
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
     </row>
-    <row r="31" ht="128.35" customHeight="1">
-      <c r="A31" s="3"/>
+    <row r="31" ht="32.35" customHeight="1">
+      <c r="A31" t="s" s="2">
+        <v>68</v>
+      </c>
       <c r="B31" t="s" s="2">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -2739,13 +2741,13 @@
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
     </row>
-    <row r="32" ht="80.35" customHeight="1">
+    <row r="32" ht="128.35" customHeight="1">
       <c r="A32" s="3"/>
       <c r="B32" t="s" s="2">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -2769,15 +2771,13 @@
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
     </row>
-    <row r="33" ht="20.35" customHeight="1">
-      <c r="A33" t="s" s="2">
-        <v>73</v>
-      </c>
+    <row r="33" ht="80.35" customHeight="1">
+      <c r="A33" s="3"/>
       <c r="B33" t="s" s="2">
-        <v>1</v>
+        <v>71</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>25</v>
+        <v>72</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -2801,13 +2801,15 @@
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
     </row>
-    <row r="34" ht="32.35" customHeight="1">
-      <c r="A34" s="3"/>
+    <row r="34" ht="20.35" customHeight="1">
+      <c r="A34" t="s" s="2">
+        <v>73</v>
+      </c>
       <c r="B34" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="C34" s="2">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C34" t="s" s="2">
+        <v>37</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -2831,13 +2833,13 @@
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
     </row>
-    <row r="35" ht="20.35" customHeight="1">
+    <row r="35" ht="32.35" customHeight="1">
       <c r="A35" s="3"/>
       <c r="B35" t="s" s="2">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C35" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -2862,13 +2864,13 @@
       <c r="X35" s="3"/>
     </row>
     <row r="36" ht="20.35" customHeight="1">
-      <c r="A36" t="s" s="2">
-        <v>76</v>
-      </c>
+      <c r="A36" s="3"/>
       <c r="B36" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C36" s="3"/>
+        <v>75</v>
+      </c>
+      <c r="C36" s="2">
+        <v>2</v>
+      </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
@@ -2891,10 +2893,12 @@
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
     </row>
-    <row r="37" ht="32.35" customHeight="1">
-      <c r="A37" s="3"/>
+    <row r="37" ht="20.35" customHeight="1">
+      <c r="A37" t="s" s="2">
+        <v>76</v>
+      </c>
       <c r="B37" t="s" s="2">
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -2919,10 +2923,10 @@
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
     </row>
-    <row r="38" ht="20.35" customHeight="1">
+    <row r="38" ht="32.35" customHeight="1">
       <c r="A38" s="3"/>
       <c r="B38" t="s" s="2">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -2950,7 +2954,7 @@
     <row r="39" ht="20.35" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" t="s" s="2">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -2976,18 +2980,12 @@
       <c r="X39" s="3"/>
     </row>
     <row r="40" ht="20.35" customHeight="1">
-      <c r="A40" t="s" s="2">
-        <v>80</v>
-      </c>
+      <c r="A40" s="3"/>
       <c r="B40" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C40" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="D40" t="s" s="2">
-        <v>81</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
@@ -3009,16 +3007,18 @@
       <c r="W40" s="3"/>
       <c r="X40" s="3"/>
     </row>
-    <row r="41" ht="32.35" customHeight="1">
-      <c r="A41" s="2"/>
+    <row r="41" ht="20.35" customHeight="1">
+      <c r="A41" t="s" s="2">
+        <v>80</v>
+      </c>
       <c r="B41" t="s" s="2">
-        <v>82</v>
+        <v>1</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>83</v>
+        <v>30</v>
       </c>
       <c r="D41" t="s" s="2">
-        <v>61</v>
+        <v>81</v>
       </c>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
@@ -3041,191 +3041,193 @@
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
     </row>
-    <row r="42" ht="56.35" customHeight="1">
-      <c r="A42" t="s" s="2">
+    <row r="42" ht="32.35" customHeight="1">
+      <c r="A42" s="2"/>
+      <c r="B42" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="C42" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="D42" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="3"/>
+      <c r="U42" s="3"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="3"/>
+      <c r="X42" s="3"/>
+    </row>
+    <row r="43" ht="56.35" customHeight="1">
+      <c r="A43" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="B42" t="s" s="2">
+      <c r="B43" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="C42" t="s" s="2">
+      <c r="C43" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D42" t="s" s="2">
+      <c r="D43" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="E42" t="s" s="2">
+      <c r="E43" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="F42" t="s" s="2">
+      <c r="F43" t="s" s="2">
         <v>87</v>
       </c>
-      <c r="G42" t="s" s="2">
+      <c r="G43" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="H42" t="s" s="2">
+      <c r="H43" t="s" s="2">
         <v>89</v>
       </c>
-      <c r="I42" t="s" s="2">
+      <c r="I43" t="s" s="2">
         <v>90</v>
       </c>
-      <c r="J42" t="s" s="2">
+      <c r="J43" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="K42" t="s" s="2">
+      <c r="K43" t="s" s="2">
         <v>92</v>
       </c>
-      <c r="L42" t="s" s="2">
+      <c r="L43" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="M42" t="s" s="2">
+      <c r="M43" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="N42" t="s" s="2">
+      <c r="N43" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="O42" t="s" s="2">
+      <c r="O43" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="P42" t="s" s="2">
+      <c r="P43" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="Q42" t="s" s="2">
+      <c r="Q43" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="R42" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="S42" t="s" s="2">
+      <c r="R43" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="S43" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="T42" t="s" s="2">
+      <c r="T43" t="s" s="2">
         <v>73</v>
       </c>
-      <c r="U42" t="s" s="2">
+      <c r="U43" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="V42" t="s" s="2">
+      <c r="V43" t="s" s="2">
         <v>100</v>
       </c>
-      <c r="W42" t="s" s="2">
+      <c r="W43" t="s" s="2">
         <v>101</v>
       </c>
-      <c r="X42" t="s" s="2">
+      <c r="X43" t="s" s="2">
         <v>102</v>
       </c>
     </row>
-    <row r="43" ht="68.35" customHeight="1">
-      <c r="A43" s="2"/>
-      <c r="B43" t="s" s="2">
+    <row r="44" ht="68.35" customHeight="1">
+      <c r="A44" s="2"/>
+      <c r="B44" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="C43" t="s" s="2">
+      <c r="C44" t="s" s="2">
         <v>104</v>
       </c>
-      <c r="D43" t="s" s="2">
+      <c r="D44" t="s" s="2">
         <v>105</v>
       </c>
-      <c r="E43" t="s" s="2">
+      <c r="E44" t="s" s="2">
         <v>106</v>
       </c>
-      <c r="F43" s="5">
+      <c r="F44" s="5">
         <v>40460</v>
       </c>
-      <c r="G43" s="5">
+      <c r="G44" s="5">
         <v>40545</v>
       </c>
-      <c r="H43" s="5">
+      <c r="H44" s="5">
         <v>40825</v>
       </c>
-      <c r="I43" t="s" s="2">
+      <c r="I44" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="J43" t="s" s="2">
+      <c r="J44" t="s" s="2">
         <v>59</v>
       </c>
-      <c r="K43" t="s" s="2">
+      <c r="K44" t="s" s="2">
         <v>59</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="L44" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="M44" t="s" s="2">
         <v>59</v>
       </c>
-      <c r="N43" t="s" s="2">
+      <c r="N44" t="s" s="2">
         <v>59</v>
       </c>
-      <c r="O43" t="s" s="2">
+      <c r="O44" t="s" s="2">
         <v>59</v>
       </c>
-      <c r="P43" t="s" s="2">
+      <c r="P44" t="s" s="2">
         <v>54</v>
       </c>
-      <c r="Q43" s="2">
+      <c r="Q44" s="2">
         <v>2</v>
       </c>
-      <c r="R43" s="2">
+      <c r="R44" s="2">
         <v>3</v>
       </c>
-      <c r="S43" s="2">
+      <c r="S44" s="2">
         <v>1</v>
       </c>
-      <c r="T43" s="2">
+      <c r="T44" s="2">
         <v>1</v>
       </c>
-      <c r="U43" t="s" s="2">
+      <c r="U44" t="s" s="2">
         <v>61</v>
       </c>
-      <c r="V43" s="2">
+      <c r="V44" s="2">
         <v>2</v>
       </c>
-      <c r="W43" s="2">
+      <c r="W44" s="2">
         <v>3</v>
       </c>
-      <c r="X43" s="2">
+      <c r="X44" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="44" ht="20.35" customHeight="1">
-      <c r="A44" t="s" s="2">
+    <row r="45" ht="20.35" customHeight="1">
+      <c r="A45" t="s" s="2">
         <v>107</v>
       </c>
-      <c r="B44" t="s" s="2">
+      <c r="B45" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="C44" t="s" s="2">
+      <c r="C45" t="s" s="2">
         <v>19</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
-      <c r="R44" s="3"/>
-      <c r="S44" s="3"/>
-      <c r="T44" s="3"/>
-      <c r="U44" s="3"/>
-      <c r="V44" s="3"/>
-      <c r="W44" s="3"/>
-      <c r="X44" s="3"/>
-    </row>
-    <row r="45" ht="44.35" customHeight="1">
-      <c r="A45" s="2"/>
-      <c r="B45" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="C45" s="2">
-        <v>1</v>
       </c>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
@@ -3249,6 +3251,36 @@
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
     </row>
+    <row r="46" ht="44.35" customHeight="1">
+      <c r="A46" s="2"/>
+      <c r="B46" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="C46" s="2">
+        <v>1</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="3"/>
+      <c r="U46" s="3"/>
+      <c r="V46" s="3"/>
+      <c r="W46" s="3"/>
+      <c r="X46" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>

<commit_message>
Updated location references to be integers
</commit_message>
<xml_diff>
--- a/testdata/sample.xlsx
+++ b/testdata/sample.xlsx
@@ -125,6 +125,9 @@
     <t>Secret Court</t>
   </si>
   <si>
+    <t>Guantanamo Bay Prison</t>
+  </si>
+  <si>
     <t>Organisations</t>
   </si>
   <si>
@@ -261,9 +264,6 @@
   </si>
   <si>
     <t>Guantanamo</t>
-  </si>
-  <si>
-    <t>Caimanera, Cuba</t>
   </si>
   <si>
     <t>Title</t>
@@ -411,7 +411,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -425,6 +425,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="59" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1678,7 +1681,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X46"/>
+  <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2281,20 +2284,18 @@
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" t="s" s="2">
+    <row r="19" ht="32.35" customHeight="1">
+      <c r="A19" s="3"/>
+      <c r="B19" t="s" s="2">
         <v>37</v>
       </c>
-      <c r="B19" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="E19" s="3"/>
+      <c r="C19" s="4">
+        <v>19.902222</v>
+      </c>
+      <c r="D19" s="4">
+        <v>-75.09889</v>
+      </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -2315,16 +2316,18 @@
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" ht="56.35" customHeight="1">
-      <c r="A20" s="3"/>
+    <row r="20" ht="20.35" customHeight="1">
+      <c r="A20" t="s" s="2">
+        <v>38</v>
+      </c>
       <c r="B20" t="s" s="2">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="C20" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="D20" s="2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D20" t="s" s="2">
+        <v>30</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -2347,16 +2350,16 @@
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
     </row>
-    <row r="21" ht="104.35" customHeight="1">
+    <row r="21" ht="56.35" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="C21" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="C21" t="s" s="2">
-        <v>41</v>
-      </c>
       <c r="D21" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -2379,16 +2382,16 @@
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
     </row>
-    <row r="22" ht="68.35" customHeight="1">
+    <row r="22" ht="104.35" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="C22" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="C22" t="s" s="2">
-        <v>43</v>
-      </c>
       <c r="D22" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -2411,40 +2414,24 @@
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
     </row>
-    <row r="23" ht="32.35" customHeight="1">
-      <c r="A23" t="s" s="2">
+    <row r="23" ht="68.35" customHeight="1">
+      <c r="A23" s="3"/>
+      <c r="B23" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="C23" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="B23" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="D23" t="s" s="2">
-        <v>46</v>
-      </c>
-      <c r="E23" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="F23" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="G23" t="s" s="2">
-        <v>49</v>
-      </c>
-      <c r="H23" t="s" s="2">
-        <v>50</v>
-      </c>
-      <c r="I23" t="s" s="2">
-        <v>37</v>
-      </c>
-      <c r="J23" t="s" s="2">
-        <v>25</v>
-      </c>
-      <c r="K23" t="s" s="2">
-        <v>30</v>
-      </c>
+      <c r="D23" s="2">
+        <v>4</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
@@ -2460,38 +2447,40 @@
       <c r="X23" s="3"/>
     </row>
     <row r="24" ht="32.35" customHeight="1">
-      <c r="A24" s="2"/>
+      <c r="A24" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="B24" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s" s="2">
+        <v>46</v>
+      </c>
+      <c r="D24" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="E24" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="F24" t="s" s="2">
+        <v>49</v>
+      </c>
+      <c r="G24" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="H24" t="s" s="2">
         <v>51</v>
       </c>
-      <c r="C24" s="5">
-        <v>29962</v>
-      </c>
-      <c r="D24" t="s" s="2">
-        <v>52</v>
-      </c>
-      <c r="E24" t="s" s="2">
-        <v>34</v>
-      </c>
-      <c r="F24" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G24" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="H24" t="s" s="2">
-        <v>55</v>
-      </c>
-      <c r="I24" s="2">
-        <v>2</v>
-      </c>
-      <c r="J24" s="2">
-        <v>1</v>
-      </c>
-      <c r="K24" s="2">
-        <v>2</v>
-      </c>
-      <c r="L24" s="2"/>
+      <c r="I24" t="s" s="2">
+        <v>38</v>
+      </c>
+      <c r="J24" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="K24" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
@@ -2505,39 +2494,39 @@
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
     </row>
-    <row r="25" ht="44.35" customHeight="1">
-      <c r="A25" s="3"/>
+    <row r="25" ht="32.35" customHeight="1">
+      <c r="A25" s="2"/>
       <c r="B25" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="C25" s="6">
+        <v>29962</v>
+      </c>
+      <c r="D25" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="E25" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="F25" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="G25" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="H25" t="s" s="2">
         <v>56</v>
       </c>
-      <c r="C25" s="5">
-        <v>26774</v>
-      </c>
-      <c r="D25" t="s" s="2">
-        <v>57</v>
-      </c>
-      <c r="E25" t="s" s="2">
-        <v>35</v>
-      </c>
-      <c r="F25" t="s" s="2">
-        <v>58</v>
-      </c>
-      <c r="G25" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="H25" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="I25" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="J25" t="s" s="2">
-        <v>61</v>
+      <c r="I25" s="2">
+        <v>2</v>
+      </c>
+      <c r="J25" s="2">
+        <v>1</v>
       </c>
       <c r="K25" s="2">
-        <v>1</v>
-      </c>
-      <c r="L25" s="3"/>
+        <v>2</v>
+      </c>
+      <c r="L25" s="2"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
@@ -2551,36 +2540,38 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" ht="56.35" customHeight="1">
+    <row r="26" ht="44.35" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26" t="s" s="2">
+        <v>57</v>
+      </c>
+      <c r="C26" s="6">
+        <v>26774</v>
+      </c>
+      <c r="D26" t="s" s="2">
+        <v>58</v>
+      </c>
+      <c r="E26" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="F26" t="s" s="2">
+        <v>59</v>
+      </c>
+      <c r="G26" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="H26" t="s" s="2">
+        <v>61</v>
+      </c>
+      <c r="I26" t="s" s="2">
         <v>62</v>
       </c>
-      <c r="C26" s="5">
-        <v>17502</v>
-      </c>
-      <c r="D26" t="s" s="2">
-        <v>63</v>
-      </c>
-      <c r="E26" t="s" s="2">
-        <v>64</v>
-      </c>
-      <c r="F26" t="s" s="2">
-        <v>53</v>
-      </c>
-      <c r="G26" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="H26" t="s" s="2">
-        <v>65</v>
-      </c>
-      <c r="I26" s="2">
-        <v>3</v>
-      </c>
-      <c r="J26" s="2">
-        <v>4</v>
-      </c>
-      <c r="K26" s="3"/>
+      <c r="J26" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1</v>
+      </c>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
@@ -2595,21 +2586,35 @@
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" ht="32.35" customHeight="1">
-      <c r="A27" t="s" s="2">
+    <row r="27" ht="56.35" customHeight="1">
+      <c r="A27" s="3"/>
+      <c r="B27" t="s" s="2">
+        <v>63</v>
+      </c>
+      <c r="C27" s="6">
+        <v>17502</v>
+      </c>
+      <c r="D27" t="s" s="2">
+        <v>64</v>
+      </c>
+      <c r="E27" t="s" s="2">
+        <v>65</v>
+      </c>
+      <c r="F27" t="s" s="2">
+        <v>54</v>
+      </c>
+      <c r="G27" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="H27" t="s" s="2">
         <v>66</v>
       </c>
-      <c r="B27" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
+      <c r="I27" s="2">
+        <v>3</v>
+      </c>
+      <c r="J27" s="2">
+        <v>4</v>
+      </c>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -2625,10 +2630,12 @@
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
     </row>
-    <row r="28" ht="20.35" customHeight="1">
-      <c r="A28" s="3"/>
-      <c r="B28" s="2">
-        <v>1</v>
+    <row r="28" ht="32.35" customHeight="1">
+      <c r="A28" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="B28" t="s" s="2">
+        <v>68</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -2656,7 +2663,7 @@
     <row r="29" ht="20.35" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -2684,7 +2691,7 @@
     <row r="30" ht="20.35" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -2709,16 +2716,12 @@
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
     </row>
-    <row r="31" ht="32.35" customHeight="1">
-      <c r="A31" t="s" s="2">
-        <v>68</v>
-      </c>
-      <c r="B31" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s" s="2">
-        <v>2</v>
-      </c>
+    <row r="31" ht="20.35" customHeight="1">
+      <c r="A31" s="3"/>
+      <c r="B31" s="2">
+        <v>3</v>
+      </c>
+      <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -2741,13 +2744,15 @@
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
     </row>
-    <row r="32" ht="128.35" customHeight="1">
-      <c r="A32" s="3"/>
+    <row r="32" ht="32.35" customHeight="1">
+      <c r="A32" t="s" s="2">
+        <v>69</v>
+      </c>
       <c r="B32" t="s" s="2">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="C32" t="s" s="2">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -2771,13 +2776,13 @@
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
     </row>
-    <row r="33" ht="80.35" customHeight="1">
+    <row r="33" ht="128.35" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" t="s" s="2">
+        <v>70</v>
+      </c>
+      <c r="C33" t="s" s="2">
         <v>71</v>
-      </c>
-      <c r="C33" t="s" s="2">
-        <v>72</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -2801,15 +2806,13 @@
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
     </row>
-    <row r="34" ht="20.35" customHeight="1">
-      <c r="A34" t="s" s="2">
+    <row r="34" ht="80.35" customHeight="1">
+      <c r="A34" s="3"/>
+      <c r="B34" t="s" s="2">
+        <v>72</v>
+      </c>
+      <c r="C34" t="s" s="2">
         <v>73</v>
-      </c>
-      <c r="B34" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s" s="2">
-        <v>37</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -2833,13 +2836,15 @@
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
     </row>
-    <row r="35" ht="32.35" customHeight="1">
-      <c r="A35" s="3"/>
+    <row r="35" ht="20.35" customHeight="1">
+      <c r="A35" t="s" s="2">
+        <v>74</v>
+      </c>
       <c r="B35" t="s" s="2">
-        <v>74</v>
-      </c>
-      <c r="C35" s="2">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="C35" t="s" s="2">
+        <v>38</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -2863,13 +2868,13 @@
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
     </row>
-    <row r="36" ht="20.35" customHeight="1">
+    <row r="36" ht="32.35" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" t="s" s="2">
         <v>75</v>
       </c>
       <c r="C36" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -2894,13 +2899,13 @@
       <c r="X36" s="3"/>
     </row>
     <row r="37" ht="20.35" customHeight="1">
-      <c r="A37" t="s" s="2">
+      <c r="A37" s="3"/>
+      <c r="B37" t="s" s="2">
         <v>76</v>
       </c>
-      <c r="B37" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3"/>
+      <c r="C37" s="2">
+        <v>2</v>
+      </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
@@ -2923,10 +2928,12 @@
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
     </row>
-    <row r="38" ht="32.35" customHeight="1">
-      <c r="A38" s="3"/>
+    <row r="38" ht="20.35" customHeight="1">
+      <c r="A38" t="s" s="2">
+        <v>77</v>
+      </c>
       <c r="B38" t="s" s="2">
-        <v>77</v>
+        <v>1</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -2951,7 +2958,7 @@
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
     </row>
-    <row r="39" ht="20.35" customHeight="1">
+    <row r="39" ht="32.35" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" t="s" s="2">
         <v>78</v>
@@ -3008,18 +3015,12 @@
       <c r="X40" s="3"/>
     </row>
     <row r="41" ht="20.35" customHeight="1">
-      <c r="A41" t="s" s="2">
+      <c r="A41" s="3"/>
+      <c r="B41" t="s" s="2">
         <v>80</v>
       </c>
-      <c r="B41" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C41" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="D41" t="s" s="2">
-        <v>81</v>
-      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
@@ -3041,16 +3042,18 @@
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
     </row>
-    <row r="42" ht="32.35" customHeight="1">
-      <c r="A42" s="2"/>
+    <row r="42" ht="20.35" customHeight="1">
+      <c r="A42" t="s" s="2">
+        <v>81</v>
+      </c>
       <c r="B42" t="s" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="D42" t="s" s="2">
         <v>82</v>
-      </c>
-      <c r="C42" t="s" s="2">
-        <v>83</v>
-      </c>
-      <c r="D42" t="s" s="2">
-        <v>61</v>
       </c>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
@@ -3073,191 +3076,193 @@
       <c r="W42" s="3"/>
       <c r="X42" s="3"/>
     </row>
-    <row r="43" ht="56.35" customHeight="1">
-      <c r="A43" t="s" s="2">
+    <row r="43" ht="20.35" customHeight="1">
+      <c r="A43" s="2"/>
+      <c r="B43" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="C43" s="2">
+        <v>5</v>
+      </c>
+      <c r="D43" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="3"/>
+      <c r="U43" s="3"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="3"/>
+      <c r="X43" s="3"/>
+    </row>
+    <row r="44" ht="56.35" customHeight="1">
+      <c r="A44" t="s" s="2">
         <v>19</v>
       </c>
-      <c r="B43" t="s" s="2">
+      <c r="B44" t="s" s="2">
         <v>84</v>
       </c>
-      <c r="C43" t="s" s="2">
+      <c r="C44" t="s" s="2">
         <v>2</v>
       </c>
-      <c r="D43" t="s" s="2">
+      <c r="D44" t="s" s="2">
         <v>85</v>
       </c>
-      <c r="E43" t="s" s="2">
+      <c r="E44" t="s" s="2">
         <v>86</v>
       </c>
-      <c r="F43" t="s" s="2">
+      <c r="F44" t="s" s="2">
         <v>87</v>
       </c>
-      <c r="G43" t="s" s="2">
+      <c r="G44" t="s" s="2">
         <v>88</v>
       </c>
-      <c r="H43" t="s" s="2">
+      <c r="H44" t="s" s="2">
         <v>89</v>
       </c>
-      <c r="I43" t="s" s="2">
+      <c r="I44" t="s" s="2">
         <v>90</v>
       </c>
-      <c r="J43" t="s" s="2">
+      <c r="J44" t="s" s="2">
         <v>91</v>
       </c>
-      <c r="K43" t="s" s="2">
+      <c r="K44" t="s" s="2">
         <v>92</v>
       </c>
-      <c r="L43" t="s" s="2">
+      <c r="L44" t="s" s="2">
         <v>93</v>
       </c>
-      <c r="M43" t="s" s="2">
+      <c r="M44" t="s" s="2">
         <v>94</v>
       </c>
-      <c r="N43" t="s" s="2">
+      <c r="N44" t="s" s="2">
         <v>95</v>
       </c>
-      <c r="O43" t="s" s="2">
+      <c r="O44" t="s" s="2">
         <v>96</v>
       </c>
-      <c r="P43" t="s" s="2">
+      <c r="P44" t="s" s="2">
         <v>97</v>
       </c>
-      <c r="Q43" t="s" s="2">
+      <c r="Q44" t="s" s="2">
         <v>98</v>
       </c>
-      <c r="R43" t="s" s="2">
+      <c r="R44" t="s" s="2">
         <v>30</v>
       </c>
-      <c r="S43" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="T43" t="s" s="2">
-        <v>73</v>
-      </c>
-      <c r="U43" t="s" s="2">
+      <c r="S44" t="s" s="2">
+        <v>81</v>
+      </c>
+      <c r="T44" t="s" s="2">
+        <v>74</v>
+      </c>
+      <c r="U44" t="s" s="2">
         <v>99</v>
       </c>
-      <c r="V43" t="s" s="2">
+      <c r="V44" t="s" s="2">
         <v>100</v>
       </c>
-      <c r="W43" t="s" s="2">
+      <c r="W44" t="s" s="2">
         <v>101</v>
       </c>
-      <c r="X43" t="s" s="2">
+      <c r="X44" t="s" s="2">
         <v>102</v>
       </c>
     </row>
-    <row r="44" ht="68.35" customHeight="1">
-      <c r="A44" s="2"/>
-      <c r="B44" t="s" s="2">
+    <row r="45" ht="68.35" customHeight="1">
+      <c r="A45" s="2"/>
+      <c r="B45" t="s" s="2">
         <v>103</v>
       </c>
-      <c r="C44" t="s" s="2">
+      <c r="C45" t="s" s="2">
         <v>104</v>
       </c>
-      <c r="D44" t="s" s="2">
+      <c r="D45" t="s" s="2">
         <v>105</v>
       </c>
-      <c r="E44" t="s" s="2">
+      <c r="E45" t="s" s="2">
         <v>106</v>
       </c>
-      <c r="F44" s="5">
+      <c r="F45" s="6">
         <v>40460</v>
       </c>
-      <c r="G44" s="5">
+      <c r="G45" s="6">
         <v>40545</v>
       </c>
-      <c r="H44" s="5">
+      <c r="H45" s="6">
         <v>40825</v>
       </c>
-      <c r="I44" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="J44" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="K44" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="L44" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="O44" t="s" s="2">
-        <v>59</v>
-      </c>
-      <c r="P44" t="s" s="2">
-        <v>54</v>
-      </c>
-      <c r="Q44" s="2">
+      <c r="I45" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="J45" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="K45" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="L45" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="O45" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="P45" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="Q45" s="2">
         <v>2</v>
       </c>
-      <c r="R44" s="2">
+      <c r="R45" s="2">
         <v>3</v>
       </c>
-      <c r="S44" s="2">
+      <c r="S45" s="2">
         <v>1</v>
       </c>
-      <c r="T44" s="2">
+      <c r="T45" s="2">
         <v>1</v>
       </c>
-      <c r="U44" t="s" s="2">
-        <v>61</v>
-      </c>
-      <c r="V44" s="2">
+      <c r="U45" t="s" s="2">
+        <v>62</v>
+      </c>
+      <c r="V45" s="2">
         <v>2</v>
       </c>
-      <c r="W44" s="2">
+      <c r="W45" s="2">
         <v>3</v>
       </c>
-      <c r="X44" s="2">
+      <c r="X45" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="45" ht="20.35" customHeight="1">
-      <c r="A45" t="s" s="2">
+    <row r="46" ht="20.35" customHeight="1">
+      <c r="A46" t="s" s="2">
         <v>107</v>
       </c>
-      <c r="B45" t="s" s="2">
+      <c r="B46" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="C45" t="s" s="2">
+      <c r="C46" t="s" s="2">
         <v>19</v>
-      </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
-      <c r="R45" s="3"/>
-      <c r="S45" s="3"/>
-      <c r="T45" s="3"/>
-      <c r="U45" s="3"/>
-      <c r="V45" s="3"/>
-      <c r="W45" s="3"/>
-      <c r="X45" s="3"/>
-    </row>
-    <row r="46" ht="44.35" customHeight="1">
-      <c r="A46" s="2"/>
-      <c r="B46" t="s" s="2">
-        <v>109</v>
-      </c>
-      <c r="C46" s="2">
-        <v>1</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
@@ -3281,6 +3286,36 @@
       <c r="W46" s="3"/>
       <c r="X46" s="3"/>
     </row>
+    <row r="47" ht="44.35" customHeight="1">
+      <c r="A47" s="2"/>
+      <c r="B47" t="s" s="2">
+        <v>109</v>
+      </c>
+      <c r="C47" s="2">
+        <v>1</v>
+      </c>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="3"/>
+      <c r="U47" s="3"/>
+      <c r="V47" s="3"/>
+      <c r="W47" s="3"/>
+      <c r="X47" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>